<commit_message>
[Update] : Item강화 로직 구현 중
Item Stack 추가 중
</commit_message>
<xml_diff>
--- a/Assets/Resources/ExcelDB/StatUpgradeDB.xlsx
+++ b/Assets/Resources/ExcelDB/StatUpgradeDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705E8146-2C7F-4B0E-AD31-893ACEF08545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31885643-3127-49CD-A880-C047FBFF93CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,14 +443,22 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.375" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -618,10 +626,45 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1">
+        <v>101</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>

</xml_diff>